<commit_message>
Fix code review issues in generate_excel_templates.py
Co-authored-by: bsafabahar <134982285+bsafabahar@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/excel_sample_data/CheckPayables_SampleData.xlsx
+++ b/excel_sample_data/CheckPayables_SampleData.xlsx
@@ -484,25 +484,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2024-11-30</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2787222</t>
+          <t>4183127</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1456811</v>
+        <v>40992046</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-11-25</t>
+          <t>2024-12-24</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>P5049</t>
+          <t>P7614</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2024-11-12 00:00:00</t>
+          <t>2024-11-30 00:00:00</t>
         </is>
       </c>
     </row>
@@ -532,25 +532,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-09-09</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5767136</t>
+          <t>8642084</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>22519877</v>
+        <v>15813907</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-09-15</t>
+          <t>2024-02-27</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>P9551</t>
+          <t>P7573</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2024-09-09 00:00:00</t>
+          <t>2024-02-14 00:00:00</t>
         </is>
       </c>
     </row>
@@ -580,25 +580,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-01-29</t>
+          <t>2024-09-28</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2928365</t>
+          <t>4019705</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>42788234</v>
+        <v>77027541</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-02-22</t>
+          <t>2024-10-21</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>P8324</t>
+          <t>P1563</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2024-01-29 00:00:00</t>
+          <t>2024-09-28 00:00:00</t>
         </is>
       </c>
     </row>
@@ -628,25 +628,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-10-28</t>
+          <t>2024-06-12</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4014248</t>
+          <t>7753758</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1172786</v>
+        <v>73789824</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-11-21</t>
+          <t>2024-07-12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>P5238</t>
+          <t>P3535</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2024-10-28 00:00:00</t>
+          <t>2024-06-12 00:00:00</t>
         </is>
       </c>
     </row>
@@ -676,25 +676,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-10-30</t>
+          <t>2024-04-17</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2683077</t>
+          <t>8768154</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>57000454</v>
+        <v>55376422</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-04-22</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>P5863</t>
+          <t>P2435</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2024-10-30 00:00:00</t>
+          <t>2024-04-17 00:00:00</t>
         </is>
       </c>
     </row>
@@ -724,25 +724,25 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-03-24</t>
+          <t>2024-05-07</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5861776</t>
+          <t>7386505</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>50670349</v>
+        <v>60023389</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-04-20</t>
+          <t>2024-05-14</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>P5790</t>
+          <t>P2222</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2024-03-24 00:00:00</t>
+          <t>2024-05-07 00:00:00</t>
         </is>
       </c>
     </row>
@@ -772,25 +772,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-06-02</t>
+          <t>2024-08-04</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4583804</t>
+          <t>9249474</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>51883743</v>
+        <v>94310474</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-06-30</t>
+          <t>2024-08-23</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>P8952</t>
+          <t>P3066</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2024-06-02 00:00:00</t>
+          <t>2024-08-04 00:00:00</t>
         </is>
       </c>
     </row>
@@ -820,25 +820,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-07-21</t>
+          <t>2024-08-11</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7595002</t>
+          <t>6011199</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>43339119</v>
+        <v>3437555</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-08-05</t>
+          <t>2024-09-04</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>P8368</t>
+          <t>P7697</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2024-07-21 00:00:00</t>
+          <t>2024-08-11 00:00:00</t>
         </is>
       </c>
     </row>
@@ -868,25 +868,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-11-24</t>
+          <t>2024-07-21</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>9288778</t>
+          <t>6092958</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>17700474</v>
+        <v>95584027</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-11-26</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>P3538</t>
+          <t>P9432</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2024-11-24 00:00:00</t>
+          <t>2024-07-21 00:00:00</t>
         </is>
       </c>
     </row>
@@ -916,25 +916,25 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-07-16</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>9199668</t>
+          <t>7443539</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>66447517</v>
+        <v>40894231</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>P3229</t>
+          <t>P1072</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2024-04-04 00:00:00</t>
+          <t>2024-07-16 00:00:00</t>
         </is>
       </c>
     </row>
@@ -964,25 +964,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024-08-23</t>
+          <t>2024-01-15</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>4162272</t>
+          <t>4141474</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>26472692</v>
+        <v>83247516</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2024-08-29</t>
+          <t>2024-02-05</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>P5667</t>
+          <t>P1947</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2024-08-23 00:00:00</t>
+          <t>2024-01-15 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1012,25 +1012,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2024-09-20</t>
+          <t>2024-08-31</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3184588</t>
+          <t>9566439</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>49918095</v>
+        <v>17722032</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2024-09-27</t>
+          <t>2024-09-09</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>P6298</t>
+          <t>P3338</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2024-09-20 00:00:00</t>
+          <t>2024-08-31 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1060,25 +1060,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2023-12-16</t>
+          <t>2024-12-13</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2649945</t>
+          <t>8952943</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>89353931</v>
+        <v>7419332</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2024-01-03</t>
+          <t>2024-12-23</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>P9808</t>
+          <t>P6955</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2023-12-16 00:00:00</t>
+          <t>2024-12-13 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1108,25 +1108,25 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024-04-19</t>
+          <t>2024-11-22</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4052791</t>
+          <t>5301824</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>32642801</v>
+        <v>92703374</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2024-04-26</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>P8553</t>
+          <t>P2433</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2024-04-19 00:00:00</t>
+          <t>2024-11-22 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1156,25 +1156,25 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-09-09</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6981831</t>
+          <t>3380871</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>31333137</v>
+        <v>73639359</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2024-04-30</t>
+          <t>2024-10-08</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>P4607</t>
+          <t>P5226</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2024-03-31 00:00:00</t>
+          <t>2024-09-09 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1204,25 +1204,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2024-04-27</t>
+          <t>2024-01-10</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1913233</t>
+          <t>9258165</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>44535701</v>
+        <v>26867927</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2024-05-23</t>
+          <t>2024-01-28</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>P4370</t>
+          <t>P6049</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2024-04-27 00:00:00</t>
+          <t>2024-01-10 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1252,25 +1252,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2024-10-27</t>
+          <t>2024-01-12</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>7223204</t>
+          <t>3887029</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>40375701</v>
+        <v>4576951</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-01-13</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>P5969</t>
+          <t>P8633</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2024-10-27 00:00:00</t>
+          <t>2024-01-12 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1300,25 +1300,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2024-05-17</t>
+          <t>2024-10-15</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2595370</t>
+          <t>1537730</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>76881045</v>
+        <v>15614090</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2024-05-30</t>
+          <t>2024-10-26</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>P9036</t>
+          <t>P7764</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2024-05-17 00:00:00</t>
+          <t>2024-10-15 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1348,25 +1348,25 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2023-12-26</t>
+          <t>2024-01-21</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5760690</t>
+          <t>4346729</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>76402925</v>
+        <v>18265219</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2024-01-12</t>
+          <t>2024-02-05</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>P9758</t>
+          <t>P5183</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2023-12-26 00:00:00</t>
+          <t>2024-01-21 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1396,25 +1396,25 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2024-08-11</t>
+          <t>2024-12-02</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8212007</t>
+          <t>7609829</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>30812759</v>
+        <v>97147569</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2024-08-13</t>
+          <t>2024-12-30</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>P3305</t>
+          <t>P7535</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2024-08-11 00:00:00</t>
+          <t>2024-12-02 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1444,25 +1444,25 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2024-02-13</t>
+          <t>2024-02-06</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>7435631</t>
+          <t>5921149</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>8432877</v>
+        <v>71377218</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2024-03-11</t>
+          <t>2024-03-03</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>P6077</t>
+          <t>P6402</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2024-02-13 00:00:00</t>
+          <t>2024-02-06 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1492,25 +1492,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2024-04-22</t>
+          <t>2024-05-31</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>5020816</t>
+          <t>4928833</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>24042525</v>
+        <v>63684591</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2024-04-28</t>
+          <t>2024-06-15</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>P8568</t>
+          <t>P4945</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2024-04-22 00:00:00</t>
+          <t>2024-05-31 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1540,25 +1540,25 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2024-02-18</t>
+          <t>2024-08-12</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>4094480</t>
+          <t>1182440</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>60898190</v>
+        <v>56954506</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2024-03-14</t>
+          <t>2024-08-25</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>P5006</t>
+          <t>P9920</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2024-02-18 00:00:00</t>
+          <t>2024-08-12 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1588,25 +1588,25 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2023-12-16</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>8465280</t>
+          <t>9531988</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>79923584</v>
+        <v>78575992</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-01-03</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>P4314</t>
+          <t>P2410</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2024-11-06 00:00:00</t>
+          <t>2023-12-16 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1636,25 +1636,25 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2024-06-05</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1026075</t>
+          <t>7019946</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>65981831</v>
+        <v>89344127</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2024-06-23</t>
+          <t>2024-12-18</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>P1626</t>
+          <t>P9536</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2024-06-05 00:00:00</t>
+          <t>2024-11-25 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1684,25 +1684,25 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2024-07-30</t>
+          <t>2024-11-27</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>8233711</t>
+          <t>9477995</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>77073721</v>
+        <v>4979798</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-12-18</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>P3545</t>
+          <t>P9641</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2024-07-30 00:00:00</t>
+          <t>2024-11-27 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1732,25 +1732,25 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2024-09-23</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8016818</t>
+          <t>5975037</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2002489</v>
+        <v>92595237</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2024-10-03</t>
+          <t>2024-08-19</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>P9790</t>
+          <t>P2877</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2024-09-23 00:00:00</t>
+          <t>2024-08-01 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1780,25 +1780,25 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2024-04-25</t>
+          <t>2024-02-25</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>8735466</t>
+          <t>2695711</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>53730825</v>
+        <v>79552956</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2024-05-19</t>
+          <t>2024-03-05</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>P8594</t>
+          <t>P4306</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2024-04-25 00:00:00</t>
+          <t>2024-02-25 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1828,25 +1828,25 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2024-11-30</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3421177</t>
+          <t>6598322</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>76115670</v>
+        <v>2143179</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2024-12-03</t>
+          <t>2024-08-10</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>P5382</t>
+          <t>P8305</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2024-11-30 00:00:00</t>
+          <t>2024-07-29 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1876,25 +1876,25 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2024-09-05</t>
+          <t>2024-03-26</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>7108906</t>
+          <t>4814825</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>50046496</v>
+        <v>6732966</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2024-09-30</t>
+          <t>2024-04-21</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>P4402</t>
+          <t>P4167</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1909,7 +1909,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2024-09-05 00:00:00</t>
+          <t>2024-03-26 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1924,25 +1924,25 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2024-03-06</t>
+          <t>2024-07-01</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2717534</t>
+          <t>6898874</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>85456994</v>
+        <v>8213680</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2024-03-22</t>
+          <t>2024-07-26</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>P8838</t>
+          <t>P2839</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2024-03-06 00:00:00</t>
+          <t>2024-07-01 00:00:00</t>
         </is>
       </c>
     </row>
@@ -1972,25 +1972,25 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2024-10-10</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>5228767</t>
+          <t>2835894</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>76007557</v>
+        <v>8839397</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2024-10-18</t>
+          <t>2024-11-15</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>P7267</t>
+          <t>P8774</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2024-10-10 00:00:00</t>
+          <t>2024-11-09 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2020,25 +2020,25 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2023-12-24</t>
+          <t>2024-06-23</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5132181</t>
+          <t>7898101</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>23944138</v>
+        <v>47133510</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2024-01-01</t>
+          <t>2024-07-19</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>P8709</t>
+          <t>P4585</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2023-12-24 00:00:00</t>
+          <t>2024-06-23 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2068,25 +2068,25 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2024-08-31</t>
+          <t>2024-02-05</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4142866</t>
+          <t>5449676</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>25798610</v>
+        <v>1823298</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2024-09-08</t>
+          <t>2024-02-18</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>P1192</t>
+          <t>P9621</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2024-08-31 00:00:00</t>
+          <t>2024-02-05 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2116,25 +2116,25 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2024-01-18</t>
+          <t>2023-12-18</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2167876</t>
+          <t>7966042</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>67859681</v>
+        <v>6222647</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2024-02-09</t>
+          <t>2024-01-07</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>P9998</t>
+          <t>P7718</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2024-01-18 00:00:00</t>
+          <t>2023-12-18 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2164,25 +2164,25 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2024-05-23</t>
+          <t>2024-10-15</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>8985643</t>
+          <t>8610063</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>34919389</v>
+        <v>61308613</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2024-06-20</t>
+          <t>2024-10-25</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>P7718</t>
+          <t>P5772</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2024-05-23 00:00:00</t>
+          <t>2024-10-15 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2212,25 +2212,25 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2024-03-14</t>
+          <t>2024-09-20</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1042054</t>
+          <t>7001931</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>89448453</v>
+        <v>90558602</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-09-30</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>P1390</t>
+          <t>P7926</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2024-03-14 00:00:00</t>
+          <t>2024-09-20 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2260,25 +2260,25 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2024-08-31</t>
+          <t>2024-03-05</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3741102</t>
+          <t>4245968</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>5191459</v>
+        <v>38363271</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2024-09-04</t>
+          <t>2024-03-26</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>P3658</t>
+          <t>P5849</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2024-08-31 00:00:00</t>
+          <t>2024-03-05 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2308,25 +2308,25 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2024-02-28</t>
+          <t>2024-12-09</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2866630</t>
+          <t>1507665</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>84949153</v>
+        <v>48023119</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2024-03-04</t>
+          <t>2024-12-25</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>P5973</t>
+          <t>P6584</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2024-02-28 00:00:00</t>
+          <t>2024-12-09 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2356,25 +2356,25 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-08-06</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1296535</t>
+          <t>2918127</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>33170056</v>
+        <v>89329245</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2024-08-29</t>
+          <t>2024-08-12</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>P7560</t>
+          <t>P6043</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2389,7 +2389,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2024-08-07 00:00:00</t>
+          <t>2024-08-06 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2404,25 +2404,25 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>6092956</t>
+          <t>5816986</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>85674622</v>
+        <v>28203546</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2024-04-21</t>
+          <t>2024-10-24</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>P2839</t>
+          <t>P2982</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2024-03-31 00:00:00</t>
+          <t>2024-09-26 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2452,25 +2452,25 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2024-07-14</t>
+          <t>2024-08-11</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>8718643</t>
+          <t>3658415</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>17380731</v>
+        <v>61135413</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2024-07-28</t>
+          <t>2024-09-05</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>P5326</t>
+          <t>P5170</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2024-07-14 00:00:00</t>
+          <t>2024-08-11 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2500,25 +2500,25 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2024-09-15</t>
+          <t>2024-06-05</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7572781</t>
+          <t>3595940</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>71350943</v>
+        <v>34427575</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2024-09-24</t>
+          <t>2024-06-26</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>P4811</t>
+          <t>P8764</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2024-09-15 00:00:00</t>
+          <t>2024-06-05 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2548,25 +2548,25 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-09-25</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>6699746</t>
+          <t>2735585</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>30701386</v>
+        <v>63172080</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2024-10-12</t>
+          <t>2024-09-27</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>P5278</t>
+          <t>P3909</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2024-10-01 00:00:00</t>
+          <t>2024-09-25 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2596,25 +2596,25 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2024-09-24</t>
+          <t>2024-03-23</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>9912943</t>
+          <t>6085865</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>51124697</v>
+        <v>42692518</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2024-10-18</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>P2941</t>
+          <t>P7225</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2024-09-24 00:00:00</t>
+          <t>2024-03-23 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2644,25 +2644,25 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2024-03-25</t>
+          <t>2024-12-03</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>7235470</t>
+          <t>8785366</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>49638944</v>
+        <v>3218558</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-12-08</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>P1514</t>
+          <t>P9230</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2024-03-25 00:00:00</t>
+          <t>2024-12-03 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2692,25 +2692,25 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2024-02-29</t>
+          <t>2024-07-01</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>8451563</t>
+          <t>9910429</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>6005525</v>
+        <v>84650229</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2024-03-02</t>
+          <t>2024-07-06</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>P5386</t>
+          <t>P2360</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2024-02-29 00:00:00</t>
+          <t>2024-07-01 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2740,25 +2740,25 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
+          <t>2024-05-02</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2257196</t>
+          <t>6603980</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>90691992</v>
+        <v>40261613</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-05-20</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>P3991</t>
+          <t>P9165</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2024-07-22 00:00:00</t>
+          <t>2024-05-02 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2788,25 +2788,25 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2024-08-17</t>
+          <t>2024-08-22</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>8177070</t>
+          <t>9588029</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>22357861</v>
+        <v>34401745</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2024-09-10</t>
+          <t>2024-09-02</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>P3518</t>
+          <t>P1574</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2024-08-17 00:00:00</t>
+          <t>2024-08-22 00:00:00</t>
         </is>
       </c>
     </row>
@@ -2836,25 +2836,25 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2024-03-13</t>
+          <t>2024-01-03</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>9412785</t>
+          <t>8199321</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>36190193</v>
+        <v>20595886</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-01-14</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>P8020</t>
+          <t>P7914</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>2024-03-13 00:00:00</t>
+          <t>2024-01-03 00:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>